<commit_message>
taraz level bug fixed, offcode edit button bug fixed
</commit_message>
<xml_diff>
--- a/public/assets/add_question_sample.xlsx
+++ b/public/assets/add_question_sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t xml:space="preserve">ردیف</t>
   </si>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">تعداد خطوط مورد نیاز</t>
   </si>
   <si>
+    <t xml:space="preserve">سال</t>
+  </si>
+  <si>
     <t xml:space="preserve">آی دی تگ</t>
   </si>
   <si>
@@ -100,6 +103,9 @@
     <t xml:space="preserve">a02</t>
   </si>
   <si>
+    <t xml:space="preserve">۱۴۰۰</t>
+  </si>
+  <si>
     <t xml:space="preserve">tag1</t>
   </si>
   <si>
@@ -107,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">a03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">۱۳۹۹</t>
   </si>
   <si>
     <t xml:space="preserve">tag3</t>
@@ -209,16 +218,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,16 +256,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.26"/>
@@ -269,7 +274,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -278,7 +283,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -314,17 +319,20 @@
       <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>14</v>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,16 +340,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="n">
         <v>8365765</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
+      <c r="D2" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>100</v>
@@ -350,22 +358,22 @@
         <v>2</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="O2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,16 +381,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="n">
         <v>8365765</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>200</v>
@@ -391,19 +399,22 @@
         <v>3</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>4</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,16 +422,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="n">
         <v>8365765</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
+      <c r="D4" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>50</v>
@@ -429,16 +440,19 @@
         <v>1</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="R4" s="0" t="s">
-        <v>29</v>
+      <c r="O4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,16 +460,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="n">
         <v>8365765</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>31</v>
+      <c r="D5" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>90</v>
@@ -464,22 +478,22 @@
         <v>4</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="O5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>22</v>
+      <c r="P5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,16 +501,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4" t="n">
         <v>8365765</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>31</v>
+      <c r="D6" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>120</v>
@@ -505,13 +519,16 @@
         <v>2</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>2011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>